<commit_message>
Added shuffle function to shuffle dataset
</commit_message>
<xml_diff>
--- a/Project1FollowUp/output.xlsx
+++ b/Project1FollowUp/output.xlsx
@@ -519,7 +519,7 @@
         <v>1</v>
       </c>
       <c r="C8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -1245,7 +1245,7 @@
         <v>1</v>
       </c>
       <c r="C74" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="75">
@@ -1410,7 +1410,7 @@
         <v>1</v>
       </c>
       <c r="C89" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="90">
@@ -2125,7 +2125,7 @@
         <v>1</v>
       </c>
       <c r="C154" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="155">
@@ -2268,7 +2268,7 @@
         <v>1</v>
       </c>
       <c r="C167" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="168">
@@ -2345,7 +2345,7 @@
         <v>1</v>
       </c>
       <c r="C174" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="175">
@@ -2411,7 +2411,7 @@
         <v>1</v>
       </c>
       <c r="C180" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="181">
@@ -2499,7 +2499,7 @@
         <v>1</v>
       </c>
       <c r="C188" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="189">
@@ -2521,7 +2521,7 @@
         <v>1</v>
       </c>
       <c r="C190" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="191">
@@ -2807,7 +2807,7 @@
         <v>1</v>
       </c>
       <c r="C216" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="217">
@@ -2917,7 +2917,7 @@
         <v>1</v>
       </c>
       <c r="C226" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="227">
@@ -2939,7 +2939,7 @@
         <v>1</v>
       </c>
       <c r="C228" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="229">
@@ -3247,7 +3247,7 @@
         <v>1</v>
       </c>
       <c r="C256" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="257">
@@ -3313,7 +3313,7 @@
         <v>1</v>
       </c>
       <c r="C262" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="263">
@@ -3324,7 +3324,7 @@
         <v>1</v>
       </c>
       <c r="C263" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="264">
@@ -3357,7 +3357,7 @@
         <v>1</v>
       </c>
       <c r="C266" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="267">
@@ -3467,7 +3467,7 @@
         <v>1</v>
       </c>
       <c r="C276" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="277">
@@ -3599,7 +3599,7 @@
         <v>1</v>
       </c>
       <c r="C288" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="289">
@@ -3665,7 +3665,7 @@
         <v>1</v>
       </c>
       <c r="C294" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="295">
@@ -3687,7 +3687,7 @@
         <v>1</v>
       </c>
       <c r="C296" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="297">
@@ -3720,7 +3720,7 @@
         <v>1</v>
       </c>
       <c r="C299" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="300">
@@ -3775,7 +3775,7 @@
         <v>1</v>
       </c>
       <c r="C304" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="305">
@@ -3797,7 +3797,7 @@
         <v>1</v>
       </c>
       <c r="C306" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="307">
@@ -3984,7 +3984,7 @@
         <v>1</v>
       </c>
       <c r="C323" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="324">
@@ -4006,7 +4006,7 @@
         <v>1</v>
       </c>
       <c r="C325" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="326">
@@ -4039,7 +4039,7 @@
         <v>1</v>
       </c>
       <c r="C328" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="329">
@@ -4050,7 +4050,7 @@
         <v>1</v>
       </c>
       <c r="C329" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="330">
@@ -4083,7 +4083,7 @@
         <v>1</v>
       </c>
       <c r="C332" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="333">
@@ -4094,7 +4094,7 @@
         <v>1</v>
       </c>
       <c r="C333" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="334">
@@ -4127,7 +4127,7 @@
         <v>1</v>
       </c>
       <c r="C336" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="337">
@@ -4160,7 +4160,7 @@
         <v>1</v>
       </c>
       <c r="C339" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="340">
@@ -4171,7 +4171,7 @@
         <v>1</v>
       </c>
       <c r="C340" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="341">
@@ -4182,7 +4182,7 @@
         <v>1</v>
       </c>
       <c r="C341" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="342">
@@ -4193,7 +4193,7 @@
         <v>1</v>
       </c>
       <c r="C342" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="343">
@@ -4215,7 +4215,7 @@
         <v>1</v>
       </c>
       <c r="C344" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="345">
@@ -4270,7 +4270,7 @@
         <v>1</v>
       </c>
       <c r="C349" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="350">
@@ -4435,7 +4435,7 @@
         <v>1</v>
       </c>
       <c r="C364" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="365">
@@ -4523,7 +4523,7 @@
         <v>1</v>
       </c>
       <c r="C372" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="373">
@@ -4567,7 +4567,7 @@
         <v>1</v>
       </c>
       <c r="C376" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="377">
@@ -4754,7 +4754,7 @@
         <v>1</v>
       </c>
       <c r="C393" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="394">
@@ -4820,7 +4820,7 @@
         <v>1</v>
       </c>
       <c r="C399" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="400">
@@ -4897,7 +4897,7 @@
         <v>1</v>
       </c>
       <c r="C406" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="407">
@@ -4930,7 +4930,7 @@
         <v>1</v>
       </c>
       <c r="C409" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="410">
@@ -4941,7 +4941,7 @@
         <v>1</v>
       </c>
       <c r="C410" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="411">
@@ -4952,7 +4952,7 @@
         <v>1</v>
       </c>
       <c r="C411" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="412">
@@ -5073,7 +5073,7 @@
         <v>1</v>
       </c>
       <c r="C422" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="423">
@@ -5106,7 +5106,7 @@
         <v>1</v>
       </c>
       <c r="C425" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="426">
@@ -5128,7 +5128,7 @@
         <v>1</v>
       </c>
       <c r="C427" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="428">
@@ -5172,7 +5172,7 @@
         <v>1</v>
       </c>
       <c r="C431" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="432">
@@ -5183,7 +5183,7 @@
         <v>1</v>
       </c>
       <c r="C432" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="433">
@@ -5194,7 +5194,7 @@
         <v>1</v>
       </c>
       <c r="C433" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="434">
@@ -5205,7 +5205,7 @@
         <v>1</v>
       </c>
       <c r="C434" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="435">
@@ -5216,7 +5216,7 @@
         <v>1</v>
       </c>
       <c r="C435" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="436">
@@ -5260,7 +5260,7 @@
         <v>1</v>
       </c>
       <c r="C439" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="440">
@@ -5271,7 +5271,7 @@
         <v>1</v>
       </c>
       <c r="C440" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="441">
@@ -5282,7 +5282,7 @@
         <v>1</v>
       </c>
       <c r="C441" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="442">
@@ -5304,7 +5304,7 @@
         <v>1</v>
       </c>
       <c r="C443" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="444">
@@ -5315,7 +5315,7 @@
         <v>1</v>
       </c>
       <c r="C444" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="445">
@@ -5326,7 +5326,7 @@
         <v>1</v>
       </c>
       <c r="C445" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="446">
@@ -5645,7 +5645,7 @@
         <v>1</v>
       </c>
       <c r="C474" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="475">
@@ -5689,7 +5689,7 @@
         <v>1</v>
       </c>
       <c r="C478" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="479">
@@ -5733,7 +5733,7 @@
         <v>1</v>
       </c>
       <c r="C482" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="483">
@@ -5909,7 +5909,7 @@
         <v>1</v>
       </c>
       <c r="C498" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="499">
@@ -5931,7 +5931,7 @@
         <v>1</v>
       </c>
       <c r="C500" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="501">
@@ -5986,7 +5986,7 @@
         <v>1</v>
       </c>
       <c r="C505" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="506">
@@ -6008,7 +6008,7 @@
         <v>1</v>
       </c>
       <c r="C507" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="508">
@@ -6019,7 +6019,7 @@
         <v>1</v>
       </c>
       <c r="C508" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="509">
@@ -6635,7 +6635,7 @@
         <v>0</v>
       </c>
       <c r="C564" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="565">
@@ -6987,7 +6987,7 @@
         <v>0</v>
       </c>
       <c r="C596" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="597">
@@ -7361,7 +7361,7 @@
         <v>0</v>
       </c>
       <c r="C630" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="631">
@@ -7427,7 +7427,7 @@
         <v>0</v>
       </c>
       <c r="C636" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="637">
@@ -7449,7 +7449,7 @@
         <v>0</v>
       </c>
       <c r="C638" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="639">
@@ -7526,7 +7526,7 @@
         <v>0</v>
       </c>
       <c r="C645" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="646">
@@ -7691,7 +7691,7 @@
         <v>0</v>
       </c>
       <c r="C660" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="661">
@@ -8076,7 +8076,7 @@
         <v>0</v>
       </c>
       <c r="C695" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="696">
@@ -8461,7 +8461,7 @@
         <v>0</v>
       </c>
       <c r="C730" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="731">
@@ -8769,7 +8769,7 @@
         <v>0</v>
       </c>
       <c r="C758" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="759">
@@ -9913,7 +9913,7 @@
         <v>0</v>
       </c>
       <c r="C862" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="863">
@@ -10298,7 +10298,7 @@
         <v>0</v>
       </c>
       <c r="C897" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="898">
@@ -11486,7 +11486,7 @@
         <v>0</v>
       </c>
       <c r="C1005" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1006">

</xml_diff>